<commit_message>
controller is no longer global. Change url to always have a search string (avoids spurious reload) Update all requirejs dependencies. Update to newer library versions. database load fix - had caused first form load to fail for linked subforms. rework how jqueryMobile is loaded.
</commit_message>
<xml_diff>
--- a/form-files/framework/framework.xlsx
+++ b/form-files/framework/framework.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="230" yWindow="560" windowWidth="23260" windowHeight="12370" activeTab="2"/>
+    <workbookView xWindow="230" yWindow="560" windowWidth="23260" windowHeight="12370" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="5" r:id="rId1"/>
@@ -166,46 +166,46 @@
     <t>url</t>
   </si>
   <si>
-    <t>opendatakit.getHashString('../tables/breathcounter/forms/breathcounter/',null)</t>
-  </si>
-  <si>
-    <t>opendatakit.getHashString('../tables/complex_validate_test/forms/complex_validate_test/',null)</t>
-  </si>
-  <si>
-    <t>opendatakit.getHashString('../tables/customAppearance/forms/customAppearance/',null)</t>
-  </si>
-  <si>
-    <t>opendatakit.getHashString('../tables/exampleForm/forms/exampleForm/',null)</t>
-  </si>
-  <si>
-    <t>opendatakit.getHashString('../tables/household/forms/household/',null)</t>
-  </si>
-  <si>
-    <t>opendatakit.getHashString('../tables/household/forms/household_new/',null)</t>
-  </si>
-  <si>
-    <t>opendatakit.getHashString('../tables/household_member/forms/household_member/',null)</t>
-  </si>
-  <si>
-    <t>opendatakit.getHashString('../tables/refrigerators/forms/refrigerators_update/',null)</t>
-  </si>
-  <si>
-    <t>opendatakit.getHashString('../tables/refrigerators/forms/refrigerators_init/',null)</t>
-  </si>
-  <si>
-    <t>opendatakit.getHashString('../tables/imnci/forms/imnci_test/',null)</t>
-  </si>
-  <si>
-    <t>opendatakit.getHashString('../tables/section_test/forms/section_test/',null)</t>
-  </si>
-  <si>
-    <t>opendatakit.getHashString('../tables/selects/forms/selects/',null)</t>
-  </si>
-  <si>
     <t>complex_validate_test</t>
   </si>
   <si>
     <t>framework</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../tables/breathcounter/forms/breathcounter/',null)</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../tables/complex_validate_test/forms/complex_validate_test/',null)</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../tables/customAppearance/forms/customAppearance/',null)</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../tables/exampleForm/forms/exampleForm/',null)</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../tables/household/forms/household/',null)</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../tables/household/forms/household_new/',null)</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../tables/household_member/forms/household_member/',null)</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../tables/imnci/forms/imnci_test/',null)</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../tables/refrigerators/forms/refrigerators_init/',null)</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../tables/refrigerators/forms/refrigerators_update/',null)</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../tables/section_test/forms/section_test/',null)</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../tables/selects/forms/selects/',null)</t>
   </si>
 </sst>
 </file>
@@ -244,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -255,6 +255,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -590,8 +593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J72"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.08984375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -699,8 +702,8 @@
     </row>
     <row r="9" spans="1:10" ht="59" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
-      <c r="B9" t="s">
-        <v>49</v>
+      <c r="B9" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="C9" t="s">
         <v>47</v>
@@ -721,14 +724,14 @@
     </row>
     <row r="11" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="B11" s="3"/>
     </row>
     <row r="12" spans="1:10" ht="59" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
-      <c r="B12" t="s">
-        <v>50</v>
+      <c r="B12" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="C12" t="s">
         <v>47</v>
@@ -755,8 +758,8 @@
     </row>
     <row r="15" spans="1:10" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
-      <c r="B15" t="s">
-        <v>51</v>
+      <c r="B15" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="C15" t="s">
         <v>47</v>
@@ -782,8 +785,8 @@
     </row>
     <row r="18" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
-      <c r="B18" t="s">
-        <v>52</v>
+      <c r="B18" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="C18" t="s">
         <v>47</v>
@@ -809,8 +812,8 @@
     </row>
     <row r="21" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
-      <c r="B21" t="s">
-        <v>53</v>
+      <c r="B21" s="4" t="s">
+        <v>55</v>
       </c>
       <c r="C21" t="s">
         <v>47</v>
@@ -836,8 +839,8 @@
     </row>
     <row r="24" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
-      <c r="B24" t="s">
-        <v>54</v>
+      <c r="B24" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="C24" t="s">
         <v>47</v>
@@ -863,8 +866,8 @@
     </row>
     <row r="27" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
-      <c r="B27" t="s">
-        <v>55</v>
+      <c r="B27" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="C27" t="s">
         <v>47</v>
@@ -890,7 +893,7 @@
     </row>
     <row r="30" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
-      <c r="B30" t="s">
+      <c r="B30" s="4" t="s">
         <v>58</v>
       </c>
       <c r="C30" t="s">
@@ -917,8 +920,8 @@
     </row>
     <row r="33" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
-      <c r="B33" t="s">
-        <v>57</v>
+      <c r="B33" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="C33" t="s">
         <v>47</v>
@@ -944,8 +947,8 @@
     </row>
     <row r="36" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
-      <c r="B36" t="s">
-        <v>56</v>
+      <c r="B36" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="C36" t="s">
         <v>47</v>
@@ -971,8 +974,8 @@
     </row>
     <row r="39" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
-      <c r="B39" t="s">
-        <v>59</v>
+      <c r="B39" s="4" t="s">
+        <v>61</v>
       </c>
       <c r="C39" t="s">
         <v>47</v>
@@ -998,8 +1001,8 @@
     </row>
     <row r="42" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
-      <c r="B42" t="s">
-        <v>60</v>
+      <c r="B42" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="C42" t="s">
         <v>47</v>
@@ -1056,7 +1059,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1085,7 +1088,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" t="s">
@@ -1217,10 +1220,10 @@
         <v>28</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Remove broken household survey. Changes to get Android working (no '?' search strings), including launch of subform.
</commit_message>
<xml_diff>
--- a/form-files/framework/framework.xlsx
+++ b/form-files/framework/framework.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="230" yWindow="560" windowWidth="23260" windowHeight="12370" activeTab="1"/>
+    <workbookView xWindow="230" yWindow="560" windowWidth="23260" windowHeight="12370" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="5" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="61">
   <si>
     <t>comments</t>
   </si>
@@ -115,9 +115,6 @@
     <t>exampleForm</t>
   </si>
   <si>
-    <t>household</t>
-  </si>
-  <si>
     <t>household_new</t>
   </si>
   <si>
@@ -182,9 +179,6 @@
   </si>
   <si>
     <t>'?' + opendatakit.getHashString('../tables/exampleForm/forms/exampleForm/',null)</t>
-  </si>
-  <si>
-    <t>'?' + opendatakit.getHashString('../tables/household/forms/household/',null)</t>
   </si>
   <si>
     <t>'?' + opendatakit.getHashString('../tables/household/forms/household_new/',null)</t>
@@ -591,10 +585,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J72"/>
+  <dimension ref="A1:J69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.08984375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -611,13 +605,13 @@
   <sheetData>
     <row r="1" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D1" t="s">
         <v>16</v>
@@ -629,7 +623,7 @@
         <v>1</v>
       </c>
       <c r="G1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H1" t="s">
         <v>6</v>
@@ -658,7 +652,7 @@
         <v>28</v>
       </c>
       <c r="H3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J3" t="b">
         <v>0</v>
@@ -691,7 +685,7 @@
     </row>
     <row r="7" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.25">
@@ -703,51 +697,51 @@
     <row r="9" spans="1:10" ht="59" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F9" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" t="s">
         <v>44</v>
-      </c>
-      <c r="H9" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="D10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B11" s="3"/>
     </row>
     <row r="12" spans="1:10" ht="59" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F12" t="s">
+        <v>43</v>
+      </c>
+      <c r="H12" t="s">
         <v>44</v>
-      </c>
-      <c r="H12" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="D13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -759,23 +753,23 @@
     <row r="15" spans="1:10" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F15" t="s">
+        <v>43</v>
+      </c>
+      <c r="H15" t="s">
         <v>44</v>
-      </c>
-      <c r="H15" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="D16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -786,23 +780,23 @@
     <row r="18" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F18" t="s">
+        <v>43</v>
+      </c>
+      <c r="H18" t="s">
         <v>44</v>
-      </c>
-      <c r="H18" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="D19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -813,23 +807,23 @@
     <row r="21" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F21" t="s">
+        <v>43</v>
+      </c>
+      <c r="H21" t="s">
         <v>44</v>
-      </c>
-      <c r="H21" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="D22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -840,23 +834,23 @@
     <row r="24" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F24" t="s">
+        <v>43</v>
+      </c>
+      <c r="H24" t="s">
         <v>44</v>
-      </c>
-      <c r="H24" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="D25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -867,23 +861,23 @@
     <row r="27" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F27" t="s">
+        <v>43</v>
+      </c>
+      <c r="H27" t="s">
         <v>44</v>
-      </c>
-      <c r="H27" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="D28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -894,23 +888,23 @@
     <row r="30" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F30" t="s">
+        <v>43</v>
+      </c>
+      <c r="H30" t="s">
         <v>44</v>
-      </c>
-      <c r="H30" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="D31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -921,23 +915,23 @@
     <row r="33" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C33" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F33" t="s">
+        <v>43</v>
+      </c>
+      <c r="H33" t="s">
         <v>44</v>
-      </c>
-      <c r="H33" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="D34" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -948,23 +942,23 @@
     <row r="36" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C36" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F36" t="s">
+        <v>43</v>
+      </c>
+      <c r="H36" t="s">
         <v>44</v>
-      </c>
-      <c r="H36" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="D37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -975,52 +969,28 @@
     <row r="39" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="B39" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C39" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F39" t="s">
+        <v>43</v>
+      </c>
+      <c r="H39" t="s">
         <v>44</v>
-      </c>
-      <c r="H39" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="D40" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="3"/>
-      <c r="B42" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C42" t="s">
-        <v>47</v>
-      </c>
-      <c r="F42" t="s">
-        <v>44</v>
-      </c>
-      <c r="H42" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="3"/>
-      <c r="B43" s="3"/>
-      <c r="D43" t="s">
-        <v>43</v>
-      </c>
-    </row>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="44" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="45" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="46" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1047,9 +1017,6 @@
     <row r="67" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="68" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="69" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="70" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="71" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="72" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1088,7 +1055,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" t="s">
@@ -1180,10 +1147,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1220,10 +1187,10 @@
         <v>28</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1323,17 +1290,6 @@
       </c>
       <c r="C12" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rename hierarchy to contents and fixed contents template
</commit_message>
<xml_diff>
--- a/form-files/framework/framework.xlsx
+++ b/form-files/framework/framework.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="230" yWindow="560" windowWidth="23260" windowHeight="12370" activeTab="3"/>
+    <workbookView xWindow="2200" yWindow="120" windowWidth="23260" windowHeight="12380" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="5" r:id="rId1"/>
@@ -12,7 +12,12 @@
     <sheet name="settings" sheetId="4" r:id="rId3"/>
     <sheet name="choices" sheetId="6" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -73,9 +78,6 @@
     <t>do section survey</t>
   </si>
   <si>
-    <t>screen.showHierarchy</t>
-  </si>
-  <si>
     <t>display.title</t>
   </si>
   <si>
@@ -200,6 +202,9 @@
   </si>
   <si>
     <t>'?' + opendatakit.getHashString('../tables/selects/forms/selects/',null)</t>
+  </si>
+  <si>
+    <t>screen.showContents</t>
   </si>
 </sst>
 </file>
@@ -555,17 +560,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="26.81640625" customWidth="1"/>
-    <col min="2" max="2" width="20.81640625" customWidth="1"/>
+    <col min="1" max="1" width="26.83203125" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -573,13 +578,18 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="19.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="19.25" customHeight="1">
       <c r="B2" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -587,43 +597,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J69"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.08984375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="88.7265625" customWidth="1"/>
+    <col min="2" max="2" width="88.6640625" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="22.26953125" customWidth="1"/>
-    <col min="5" max="5" width="46.08984375" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" customWidth="1"/>
+    <col min="5" max="5" width="46.1640625" customWidth="1"/>
     <col min="6" max="7" width="20" customWidth="1"/>
-    <col min="8" max="8" width="21.81640625" customWidth="1"/>
-    <col min="9" max="9" width="31.453125" customWidth="1"/>
-    <col min="10" max="10" width="22.08984375" customWidth="1"/>
+    <col min="8" max="8" width="21.83203125" customWidth="1"/>
+    <col min="9" max="9" width="31.5" customWidth="1"/>
+    <col min="10" max="10" width="22.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="17.5" customHeight="1">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D1" t="s">
         <v>16</v>
       </c>
       <c r="E1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>
       </c>
       <c r="G1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H1" t="s">
         <v>6</v>
@@ -632,39 +640,39 @@
         <v>15</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="17" customHeight="1">
       <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
         <v>21</v>
       </c>
-      <c r="E2" t="s">
-        <v>22</v>
-      </c>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="17.5" customHeight="1">
       <c r="F3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="17" customHeight="1">
       <c r="D4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10" ht="41" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="41" customHeight="1">
       <c r="F5" t="s">
         <v>2</v>
       </c>
@@ -678,347 +686,352 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="17" customHeight="1">
       <c r="D6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="17" customHeight="1">
       <c r="D7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="17" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8" s="3"/>
     </row>
-    <row r="9" spans="1:10" ht="59" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="59" customHeight="1">
       <c r="A9" s="3"/>
       <c r="B9" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F9" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9" t="s">
         <v>43</v>
       </c>
-      <c r="H9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:10" ht="17" customHeight="1">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="D10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="17.5" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="1:10" ht="59" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="59" customHeight="1">
       <c r="A12" s="3"/>
       <c r="B12" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F12" t="s">
+        <v>42</v>
+      </c>
+      <c r="H12" t="s">
         <v>43</v>
       </c>
-      <c r="H12" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:10" ht="17" customHeight="1">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="D13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="17.5" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" s="3"/>
     </row>
-    <row r="15" spans="1:10" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="66" customHeight="1">
       <c r="A15" s="3"/>
       <c r="B15" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F15" t="s">
+        <v>42</v>
+      </c>
+      <c r="H15" t="s">
         <v>43</v>
       </c>
-      <c r="H15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:10" ht="17" customHeight="1">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="D16" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="17.5" customHeight="1">
       <c r="A17" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="66" customHeight="1">
       <c r="A18" s="3"/>
       <c r="B18" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F18" t="s">
+        <v>42</v>
+      </c>
+      <c r="H18" t="s">
         <v>43</v>
       </c>
-      <c r="H18" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:8" ht="17" customHeight="1">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="D19" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="17.5" customHeight="1">
       <c r="A20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="66" customHeight="1">
       <c r="A21" s="3"/>
       <c r="B21" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F21" t="s">
+        <v>42</v>
+      </c>
+      <c r="H21" t="s">
         <v>43</v>
       </c>
-      <c r="H21" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:8" ht="17" customHeight="1">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="D22" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="17.5" customHeight="1">
       <c r="A23" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="66" customHeight="1">
       <c r="A24" s="3"/>
       <c r="B24" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F24" t="s">
+        <v>42</v>
+      </c>
+      <c r="H24" t="s">
         <v>43</v>
       </c>
-      <c r="H24" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:8" ht="17" customHeight="1">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="D25" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="17.5" customHeight="1">
       <c r="A26" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="66" customHeight="1">
       <c r="A27" s="3"/>
       <c r="B27" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C27" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F27" t="s">
+        <v>42</v>
+      </c>
+      <c r="H27" t="s">
         <v>43</v>
       </c>
-      <c r="H27" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:8" ht="17" customHeight="1">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="D28" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="17.5" customHeight="1">
       <c r="A29" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="66" customHeight="1">
       <c r="A30" s="3"/>
       <c r="B30" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F30" t="s">
+        <v>42</v>
+      </c>
+      <c r="H30" t="s">
         <v>43</v>
       </c>
-      <c r="H30" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:8" ht="17" customHeight="1">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="D31" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="17.5" customHeight="1">
       <c r="A32" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="66" customHeight="1">
       <c r="A33" s="3"/>
       <c r="B33" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C33" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F33" t="s">
+        <v>42</v>
+      </c>
+      <c r="H33" t="s">
         <v>43</v>
       </c>
-      <c r="H33" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:8" ht="17" customHeight="1">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="D34" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="17.5" customHeight="1">
       <c r="A35" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="66" customHeight="1">
       <c r="A36" s="3"/>
       <c r="B36" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F36" t="s">
+        <v>42</v>
+      </c>
+      <c r="H36" t="s">
         <v>43</v>
       </c>
-      <c r="H36" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:8" ht="17" customHeight="1">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="D37" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="17.5" customHeight="1">
       <c r="A38" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="66" customHeight="1">
       <c r="A39" s="3"/>
       <c r="B39" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C39" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F39" t="s">
+        <v>42</v>
+      </c>
+      <c r="H39" t="s">
         <v>43</v>
       </c>
-      <c r="H39" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:8" ht="17" customHeight="1">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="D40" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="65" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="66" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="67" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="68" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="69" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="17.5" customHeight="1"/>
+    <row r="42" spans="1:8" ht="17.5" customHeight="1"/>
+    <row r="43" spans="1:8" ht="17.5" customHeight="1"/>
+    <row r="44" spans="1:8" ht="17.5" customHeight="1"/>
+    <row r="45" spans="1:8" ht="17.5" customHeight="1"/>
+    <row r="46" spans="1:8" ht="17.5" customHeight="1"/>
+    <row r="47" spans="1:8" ht="17.5" customHeight="1"/>
+    <row r="48" spans="1:8" ht="17.5" customHeight="1"/>
+    <row r="49" ht="17.5" customHeight="1"/>
+    <row r="50" ht="17.5" customHeight="1"/>
+    <row r="51" ht="17.5" customHeight="1"/>
+    <row r="52" ht="17.5" customHeight="1"/>
+    <row r="53" ht="17.5" customHeight="1"/>
+    <row r="54" ht="17.5" customHeight="1"/>
+    <row r="55" ht="17.5" customHeight="1"/>
+    <row r="56" ht="17.5" customHeight="1"/>
+    <row r="57" ht="17.5" customHeight="1"/>
+    <row r="58" ht="17.5" customHeight="1"/>
+    <row r="59" ht="17.5" customHeight="1"/>
+    <row r="60" ht="17.5" customHeight="1"/>
+    <row r="61" ht="17.5" customHeight="1"/>
+    <row r="62" ht="17.5" customHeight="1"/>
+    <row r="63" ht="17.5" customHeight="1"/>
+    <row r="64" ht="17.5" customHeight="1"/>
+    <row r="65" ht="17.5" customHeight="1"/>
+    <row r="66" ht="17.5" customHeight="1"/>
+    <row r="67" ht="17.5" customHeight="1"/>
+    <row r="68" ht="17.5" customHeight="1"/>
+    <row r="69" ht="17.5" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1030,13 +1043,13 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.08984375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="3" width="24.6328125" customWidth="1"/>
-    <col min="4" max="4" width="41.36328125" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" customWidth="1"/>
+    <col min="4" max="4" width="41.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="18.75" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -1044,25 +1057,25 @@
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="18.75" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="18.75" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1073,7 +1086,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="28" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="28" customHeight="1">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1084,64 +1097,69 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="18.75" customHeight="1">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:4" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="18.75" customHeight="1">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:4" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:4" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:4" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="18.75" customHeight="1"/>
+    <row r="8" spans="1:4" ht="18.75" customHeight="1"/>
+    <row r="9" spans="1:4" ht="18.75" customHeight="1">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:4" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="18.75" customHeight="1">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:4" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="18.75" customHeight="1">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:4" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="18.75" customHeight="1">
       <c r="A12" s="1"/>
     </row>
-    <row r="15" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="12.75" customHeight="1">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="12.75" customHeight="1">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="12.75" customHeight="1">
       <c r="A17" s="1"/>
     </row>
-    <row r="18" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="12.75" customHeight="1">
       <c r="A18" s="1"/>
     </row>
-    <row r="21" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="12.75" customHeight="1">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="12.75" customHeight="1">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="12.75" customHeight="1">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="12.75" customHeight="1">
       <c r="A24" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1153,146 +1171,151 @@
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.453125" customWidth="1"/>
-    <col min="2" max="2" width="22.36328125" customWidth="1"/>
+    <col min="1" max="1" width="18.5" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" customWidth="1"/>
     <col min="3" max="3" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="3" t="s">
+    <row r="5" spans="1:3">
+      <c r="A5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="6" spans="1:3">
+      <c r="A6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
         <v>31</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="7" spans="1:3">
+      <c r="A7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
         <v>32</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="8" spans="1:3">
+      <c r="A8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
         <v>33</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" t="s">
+    <row r="9" spans="1:3">
+      <c r="A9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
         <v>34</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="10" spans="1:3">
+      <c r="A10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
         <v>35</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="11" spans="1:3">
+      <c r="A11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
         <v>36</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" t="s">
+    <row r="12" spans="1:3">
+      <c r="A12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" t="s">
         <v>37</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add two-column screen example.
</commit_message>
<xml_diff>
--- a/form-files/framework/framework.xlsx
+++ b/form-files/framework/framework.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2200" yWindow="120" windowWidth="23260" windowHeight="12380" activeTab="3"/>
+    <workbookView xWindow="2200" yWindow="120" windowWidth="23260" windowHeight="12380" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="5" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="63">
   <si>
     <t>comments</t>
   </si>
@@ -205,6 +205,12 @@
   </si>
   <si>
     <t>screen.showContents</t>
+  </si>
+  <si>
+    <t>twoColumn</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../tables/twoColumn/forms/twoColumn/',null)</t>
   </si>
 </sst>
 </file>
@@ -564,13 +570,13 @@
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.83203125" customWidth="1"/>
-    <col min="2" max="2" width="20.83203125" customWidth="1"/>
+    <col min="1" max="1" width="26.81640625" customWidth="1"/>
+    <col min="2" max="2" width="20.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -578,7 +584,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="19.25" customHeight="1">
+    <row r="2" spans="1:2" ht="19.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>17</v>
       </c>
@@ -597,21 +603,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J69"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="17.1796875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="88.6640625" customWidth="1"/>
+    <col min="2" max="2" width="88.6328125" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="22.33203125" customWidth="1"/>
-    <col min="5" max="5" width="46.1640625" customWidth="1"/>
+    <col min="4" max="4" width="22.36328125" customWidth="1"/>
+    <col min="5" max="5" width="46.1796875" customWidth="1"/>
     <col min="6" max="7" width="20" customWidth="1"/>
-    <col min="8" max="8" width="21.83203125" customWidth="1"/>
-    <col min="9" max="9" width="31.5" customWidth="1"/>
-    <col min="10" max="10" width="22.1640625" customWidth="1"/>
+    <col min="8" max="8" width="21.81640625" customWidth="1"/>
+    <col min="9" max="9" width="31.453125" customWidth="1"/>
+    <col min="10" max="10" width="22.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17.5" customHeight="1">
+    <row r="1" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -643,7 +651,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="17" customHeight="1">
+    <row r="2" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
         <v>20</v>
       </c>
@@ -652,7 +660,7 @@
       </c>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" ht="17.5" customHeight="1">
+    <row r="3" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F3" t="s">
         <v>24</v>
       </c>
@@ -666,13 +674,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="17" customHeight="1">
+    <row r="4" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>22</v>
       </c>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10" ht="41" customHeight="1">
+    <row r="5" spans="1:10" ht="41" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F5" t="s">
         <v>2</v>
       </c>
@@ -686,23 +694,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="17" customHeight="1">
+    <row r="6" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="17" customHeight="1">
+    <row r="7" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="17" customHeight="1">
+    <row r="8" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B8" s="3"/>
     </row>
-    <row r="9" spans="1:10" ht="59" customHeight="1">
+    <row r="9" spans="1:10" ht="59" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="4" t="s">
         <v>49</v>
@@ -717,20 +725,20 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="17" customHeight="1">
+    <row r="10" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="D10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="17.5" customHeight="1">
+    <row r="11" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="1:10" ht="59" customHeight="1">
+    <row r="12" spans="1:10" ht="59" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="4" t="s">
         <v>50</v>
@@ -745,20 +753,20 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="17" customHeight="1">
+    <row r="13" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="D13" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="17.5" customHeight="1">
+    <row r="14" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B14" s="3"/>
     </row>
-    <row r="15" spans="1:10" ht="66" customHeight="1">
+    <row r="15" spans="1:10" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="4" t="s">
         <v>51</v>
@@ -773,19 +781,19 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="17" customHeight="1">
+    <row r="16" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="D16" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="17.5" customHeight="1">
+    <row r="17" spans="1:8" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="66" customHeight="1">
+    <row r="18" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="4" t="s">
         <v>52</v>
@@ -800,19 +808,19 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="17" customHeight="1">
+    <row r="19" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="D19" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="17.5" customHeight="1">
+    <row r="20" spans="1:8" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="66" customHeight="1">
+    <row r="21" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="4" t="s">
         <v>53</v>
@@ -827,19 +835,19 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="17" customHeight="1">
+    <row r="22" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="D22" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="17.5" customHeight="1">
+    <row r="23" spans="1:8" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="66" customHeight="1">
+    <row r="24" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="4" t="s">
         <v>54</v>
@@ -854,19 +862,19 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="17" customHeight="1">
+    <row r="25" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="D25" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="17.5" customHeight="1">
+    <row r="26" spans="1:8" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="66" customHeight="1">
+    <row r="27" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="4" t="s">
         <v>55</v>
@@ -881,19 +889,19 @@
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="17" customHeight="1">
+    <row r="28" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="D28" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="17.5" customHeight="1">
+    <row r="29" spans="1:8" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="66" customHeight="1">
+    <row r="30" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="4" t="s">
         <v>56</v>
@@ -908,19 +916,19 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="17" customHeight="1">
+    <row r="31" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="D31" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="17.5" customHeight="1">
+    <row r="32" spans="1:8" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="66" customHeight="1">
+    <row r="33" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="4" t="s">
         <v>57</v>
@@ -935,19 +943,19 @@
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="17" customHeight="1">
+    <row r="34" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="D34" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="17.5" customHeight="1">
+    <row r="35" spans="1:8" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="66" customHeight="1">
+    <row r="36" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="4" t="s">
         <v>58</v>
@@ -962,19 +970,19 @@
         <v>43</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="17" customHeight="1">
+    <row r="37" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="D37" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="17.5" customHeight="1">
+    <row r="38" spans="1:8" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="66" customHeight="1">
+    <row r="39" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="B39" s="4" t="s">
         <v>59</v>
@@ -989,42 +997,66 @@
         <v>43</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="17" customHeight="1">
+    <row r="40" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="D40" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="17.5" customHeight="1"/>
-    <row r="42" spans="1:8" ht="17.5" customHeight="1"/>
-    <row r="43" spans="1:8" ht="17.5" customHeight="1"/>
-    <row r="44" spans="1:8" ht="17.5" customHeight="1"/>
-    <row r="45" spans="1:8" ht="17.5" customHeight="1"/>
-    <row r="46" spans="1:8" ht="17.5" customHeight="1"/>
-    <row r="47" spans="1:8" ht="17.5" customHeight="1"/>
-    <row r="48" spans="1:8" ht="17.5" customHeight="1"/>
-    <row r="49" ht="17.5" customHeight="1"/>
-    <row r="50" ht="17.5" customHeight="1"/>
-    <row r="51" ht="17.5" customHeight="1"/>
-    <row r="52" ht="17.5" customHeight="1"/>
-    <row r="53" ht="17.5" customHeight="1"/>
-    <row r="54" ht="17.5" customHeight="1"/>
-    <row r="55" ht="17.5" customHeight="1"/>
-    <row r="56" ht="17.5" customHeight="1"/>
-    <row r="57" ht="17.5" customHeight="1"/>
-    <row r="58" ht="17.5" customHeight="1"/>
-    <row r="59" ht="17.5" customHeight="1"/>
-    <row r="60" ht="17.5" customHeight="1"/>
-    <row r="61" ht="17.5" customHeight="1"/>
-    <row r="62" ht="17.5" customHeight="1"/>
-    <row r="63" ht="17.5" customHeight="1"/>
-    <row r="64" ht="17.5" customHeight="1"/>
-    <row r="65" ht="17.5" customHeight="1"/>
-    <row r="66" ht="17.5" customHeight="1"/>
-    <row r="67" ht="17.5" customHeight="1"/>
-    <row r="68" ht="17.5" customHeight="1"/>
-    <row r="69" ht="17.5" customHeight="1"/>
+    <row r="41" spans="1:8" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="3"/>
+      <c r="B42" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C42" t="s">
+        <v>45</v>
+      </c>
+      <c r="F42" t="s">
+        <v>42</v>
+      </c>
+      <c r="H42" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="3"/>
+      <c r="B43" s="3"/>
+      <c r="D43" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:8" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:8" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:8" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:8" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1043,13 +1075,13 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="17.1796875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="24.6640625" customWidth="1"/>
-    <col min="4" max="4" width="41.33203125" customWidth="1"/>
+    <col min="3" max="3" width="24.6328125" customWidth="1"/>
+    <col min="4" max="4" width="41.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" customHeight="1">
+    <row r="1" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -1063,7 +1095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="18.75" customHeight="1">
+    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1075,7 +1107,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18.75" customHeight="1">
+    <row r="3" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1086,7 +1118,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="28" customHeight="1">
+    <row r="4" spans="1:4" ht="28" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1097,60 +1129,60 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="18.75" customHeight="1">
+    <row r="5" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:4" ht="18.75" customHeight="1">
+    <row r="6" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:4" ht="18.75" customHeight="1"/>
-    <row r="8" spans="1:4" ht="18.75" customHeight="1"/>
-    <row r="9" spans="1:4" ht="18.75" customHeight="1">
+    <row r="7" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:4" ht="18.75" customHeight="1">
+    <row r="10" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:4" ht="18.75" customHeight="1">
+    <row r="11" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:4" ht="18.75" customHeight="1">
+    <row r="12" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
     </row>
-    <row r="15" spans="1:4" ht="12.75" customHeight="1">
+    <row r="15" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:4" ht="12.75" customHeight="1">
+    <row r="16" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:3" ht="12.75" customHeight="1">
+    <row r="17" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
     </row>
-    <row r="18" spans="1:3" ht="12.75" customHeight="1">
+    <row r="18" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
     </row>
-    <row r="21" spans="1:3" ht="12.75" customHeight="1">
+    <row r="21" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="1:3" ht="12.75" customHeight="1">
+    <row r="22" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:3" ht="12.75" customHeight="1">
+    <row r="23" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:3" ht="12.75" customHeight="1">
+    <row r="24" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
     </row>
   </sheetData>
@@ -1165,20 +1197,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" customWidth="1"/>
+    <col min="1" max="1" width="18.453125" customWidth="1"/>
+    <col min="2" max="2" width="22.36328125" customWidth="1"/>
     <col min="3" max="3" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -1189,7 +1221,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>27</v>
       </c>
@@ -1200,7 +1232,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>27</v>
       </c>
@@ -1211,7 +1243,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>27</v>
       </c>
@@ -1222,7 +1254,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>27</v>
       </c>
@@ -1233,7 +1265,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>27</v>
       </c>
@@ -1244,7 +1276,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>27</v>
       </c>
@@ -1255,7 +1287,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>27</v>
       </c>
@@ -1266,7 +1298,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>27</v>
       </c>
@@ -1277,7 +1309,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>27</v>
       </c>
@@ -1288,7 +1320,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>27</v>
       </c>
@@ -1299,7 +1331,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>27</v>
       </c>
@@ -1308,6 +1340,17 @@
       </c>
       <c r="C12" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
disabled Contents popup menu item for Common Javascript Framework screen
</commit_message>
<xml_diff>
--- a/form-files/framework/framework.xlsx
+++ b/form-files/framework/framework.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2200" yWindow="120" windowWidth="23260" windowHeight="12380" activeTab="1"/>
+    <workbookView xWindow="1780" yWindow="0" windowWidth="26020" windowHeight="14080"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="5" r:id="rId1"/>
@@ -204,13 +204,13 @@
     <t>'?' + opendatakit.getHashString('../tables/selects/forms/selects/',null)</t>
   </si>
   <si>
-    <t>screen.showContents</t>
-  </si>
-  <si>
     <t>twoColumn</t>
   </si>
   <si>
     <t>'?' + opendatakit.getHashString('../tables/twoColumn/forms/twoColumn/',null)</t>
+  </si>
+  <si>
+    <t>showContents</t>
   </si>
 </sst>
 </file>
@@ -566,17 +566,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="26.81640625" customWidth="1"/>
-    <col min="2" max="2" width="20.81640625" customWidth="1"/>
+    <col min="1" max="1" width="26.83203125" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -584,7 +584,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="19.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="19.25" customHeight="1">
       <c r="B2" t="s">
         <v>17</v>
       </c>
@@ -603,23 +603,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.1796875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="88.6328125" customWidth="1"/>
+    <col min="2" max="2" width="88.6640625" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="22.36328125" customWidth="1"/>
-    <col min="5" max="5" width="46.1796875" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" customWidth="1"/>
+    <col min="5" max="5" width="46.1640625" customWidth="1"/>
     <col min="6" max="7" width="20" customWidth="1"/>
-    <col min="8" max="8" width="21.81640625" customWidth="1"/>
-    <col min="9" max="9" width="31.453125" customWidth="1"/>
-    <col min="10" max="10" width="22.1796875" customWidth="1"/>
+    <col min="8" max="8" width="21.83203125" customWidth="1"/>
+    <col min="9" max="9" width="31.5" customWidth="1"/>
+    <col min="10" max="10" width="22.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="17.5" customHeight="1">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -647,11 +647,9 @@
       <c r="I1" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J1" s="2"/>
+    </row>
+    <row r="2" spans="1:10" ht="17" customHeight="1">
       <c r="D2" t="s">
         <v>20</v>
       </c>
@@ -660,7 +658,7 @@
       </c>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="17.5" customHeight="1">
       <c r="F3" t="s">
         <v>24</v>
       </c>
@@ -670,17 +668,14 @@
       <c r="H3" t="s">
         <v>40</v>
       </c>
-      <c r="J3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:10" ht="17" customHeight="1">
       <c r="D4" t="s">
         <v>22</v>
       </c>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10" ht="41" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="41" customHeight="1">
       <c r="F5" t="s">
         <v>2</v>
       </c>
@@ -690,27 +685,24 @@
       <c r="I5" t="s">
         <v>13</v>
       </c>
-      <c r="J5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:10" ht="17" customHeight="1">
       <c r="D6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="17" customHeight="1">
       <c r="D7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="17" customHeight="1">
       <c r="A8" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B8" s="3"/>
     </row>
-    <row r="9" spans="1:10" ht="59" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="59" customHeight="1">
       <c r="A9" s="3"/>
       <c r="B9" s="4" t="s">
         <v>49</v>
@@ -725,20 +717,20 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="17" customHeight="1">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="D10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="17.5" customHeight="1">
       <c r="A11" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="1:10" ht="59" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="59" customHeight="1">
       <c r="A12" s="3"/>
       <c r="B12" s="4" t="s">
         <v>50</v>
@@ -753,20 +745,20 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="17" customHeight="1">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="D13" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="17.5" customHeight="1">
       <c r="A14" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B14" s="3"/>
     </row>
-    <row r="15" spans="1:10" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="66" customHeight="1">
       <c r="A15" s="3"/>
       <c r="B15" s="4" t="s">
         <v>51</v>
@@ -781,19 +773,19 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="17" customHeight="1">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="D16" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="17.5" customHeight="1">
       <c r="A17" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="66" customHeight="1">
       <c r="A18" s="3"/>
       <c r="B18" s="4" t="s">
         <v>52</v>
@@ -808,19 +800,19 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="17" customHeight="1">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="D19" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="17.5" customHeight="1">
       <c r="A20" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="66" customHeight="1">
       <c r="A21" s="3"/>
       <c r="B21" s="4" t="s">
         <v>53</v>
@@ -835,19 +827,19 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="17" customHeight="1">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="D22" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="17.5" customHeight="1">
       <c r="A23" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="66" customHeight="1">
       <c r="A24" s="3"/>
       <c r="B24" s="4" t="s">
         <v>54</v>
@@ -862,19 +854,19 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="17" customHeight="1">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="D25" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="17.5" customHeight="1">
       <c r="A26" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="66" customHeight="1">
       <c r="A27" s="3"/>
       <c r="B27" s="4" t="s">
         <v>55</v>
@@ -889,19 +881,19 @@
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="17" customHeight="1">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="D28" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="17.5" customHeight="1">
       <c r="A29" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="66" customHeight="1">
       <c r="A30" s="3"/>
       <c r="B30" s="4" t="s">
         <v>56</v>
@@ -916,19 +908,19 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="17" customHeight="1">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="D31" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="17.5" customHeight="1">
       <c r="A32" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="66" customHeight="1">
       <c r="A33" s="3"/>
       <c r="B33" s="4" t="s">
         <v>57</v>
@@ -943,19 +935,19 @@
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="17" customHeight="1">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="D34" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="17.5" customHeight="1">
       <c r="A35" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="66" customHeight="1">
       <c r="A36" s="3"/>
       <c r="B36" s="4" t="s">
         <v>58</v>
@@ -970,19 +962,19 @@
         <v>43</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="17" customHeight="1">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="D37" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="17.5" customHeight="1">
       <c r="A38" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="66" customHeight="1">
       <c r="A39" s="3"/>
       <c r="B39" s="4" t="s">
         <v>59</v>
@@ -997,22 +989,22 @@
         <v>43</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="17" customHeight="1">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="D40" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="17.5" customHeight="1">
       <c r="A41" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="66" customHeight="1">
       <c r="A42" s="3"/>
       <c r="B42" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C42" t="s">
         <v>45</v>
@@ -1024,39 +1016,39 @@
         <v>43</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="17" customHeight="1">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="D43" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:8" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="1:8" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:8" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:8" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="65" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="66" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="67" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="68" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="69" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:8" ht="17.5" customHeight="1"/>
+    <row r="45" spans="1:8" ht="17.5" customHeight="1"/>
+    <row r="46" spans="1:8" ht="17.5" customHeight="1"/>
+    <row r="47" spans="1:8" ht="17.5" customHeight="1"/>
+    <row r="48" spans="1:8" ht="17.5" customHeight="1"/>
+    <row r="49" ht="17.5" customHeight="1"/>
+    <row r="50" ht="17.5" customHeight="1"/>
+    <row r="51" ht="17.5" customHeight="1"/>
+    <row r="52" ht="17.5" customHeight="1"/>
+    <row r="53" ht="17.5" customHeight="1"/>
+    <row r="54" ht="17.5" customHeight="1"/>
+    <row r="55" ht="17.5" customHeight="1"/>
+    <row r="56" ht="17.5" customHeight="1"/>
+    <row r="57" ht="17.5" customHeight="1"/>
+    <row r="58" ht="17.5" customHeight="1"/>
+    <row r="59" ht="17.5" customHeight="1"/>
+    <row r="60" ht="17.5" customHeight="1"/>
+    <row r="61" ht="17.5" customHeight="1"/>
+    <row r="62" ht="17.5" customHeight="1"/>
+    <row r="63" ht="17.5" customHeight="1"/>
+    <row r="64" ht="17.5" customHeight="1"/>
+    <row r="65" ht="17.5" customHeight="1"/>
+    <row r="66" ht="17.5" customHeight="1"/>
+    <row r="67" ht="17.5" customHeight="1"/>
+    <row r="68" ht="17.5" customHeight="1"/>
+    <row r="69" ht="17.5" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1069,19 +1061,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.1796875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="3" width="24.6328125" customWidth="1"/>
-    <col min="4" max="4" width="41.36328125" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" customWidth="1"/>
+    <col min="4" max="4" width="41.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="18.75" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -1094,8 +1086,11 @@
       <c r="D1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="18.75" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1107,7 +1102,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="18.75" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1118,7 +1113,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="28" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="28" customHeight="1">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1128,61 +1123,64 @@
       <c r="D4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="18.75" customHeight="1">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="18.75" customHeight="1">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="18.75" customHeight="1"/>
+    <row r="8" spans="1:5" ht="18.75" customHeight="1"/>
+    <row r="9" spans="1:5" ht="18.75" customHeight="1">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="18.75" customHeight="1">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="18.75" customHeight="1">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="18.75" customHeight="1">
       <c r="A12" s="1"/>
     </row>
-    <row r="15" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="12.75" customHeight="1">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="12.75" customHeight="1">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="12.75" customHeight="1">
       <c r="A17" s="1"/>
     </row>
-    <row r="18" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="12.75" customHeight="1">
       <c r="A18" s="1"/>
     </row>
-    <row r="21" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="12.75" customHeight="1">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="12.75" customHeight="1">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="12.75" customHeight="1">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="12.75" customHeight="1">
       <c r="A24" s="1"/>
     </row>
   </sheetData>
@@ -1203,14 +1201,14 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.453125" customWidth="1"/>
-    <col min="2" max="2" width="22.36328125" customWidth="1"/>
+    <col min="1" max="1" width="18.5" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" customWidth="1"/>
     <col min="3" max="3" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -1221,7 +1219,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
         <v>27</v>
       </c>
@@ -1232,7 +1230,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="3" t="s">
         <v>27</v>
       </c>
@@ -1243,7 +1241,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="3" t="s">
         <v>27</v>
       </c>
@@ -1254,7 +1252,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
         <v>27</v>
       </c>
@@ -1265,7 +1263,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" s="3" t="s">
         <v>27</v>
       </c>
@@ -1276,7 +1274,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" s="3" t="s">
         <v>27</v>
       </c>
@@ -1287,7 +1285,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" s="3" t="s">
         <v>27</v>
       </c>
@@ -1298,7 +1296,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" s="3" t="s">
         <v>27</v>
       </c>
@@ -1309,7 +1307,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" s="3" t="s">
         <v>27</v>
       </c>
@@ -1320,7 +1318,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" s="3" t="s">
         <v>27</v>
       </c>
@@ -1331,7 +1329,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" s="3" t="s">
         <v>27</v>
       </c>
@@ -1342,15 +1340,15 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="A13" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove cell_type usage. Add expression sanity checking to XLSXconverter -- obviously bad formulas will be detected early.
</commit_message>
<xml_diff>
--- a/form-files/framework/framework.xlsx
+++ b/form-files/framework/framework.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1780" yWindow="0" windowWidth="26020" windowHeight="14080"/>
+    <workbookView xWindow="1780" yWindow="0" windowWidth="25820" windowHeight="14080" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="5" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="61">
   <si>
     <t>comments</t>
   </si>
@@ -154,12 +154,6 @@
   </si>
   <si>
     <t>Open form</t>
-  </si>
-  <si>
-    <t>url.cell_type</t>
-  </si>
-  <si>
-    <t>formula</t>
   </si>
   <si>
     <t>url</t>
@@ -566,17 +560,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.83203125" customWidth="1"/>
-    <col min="2" max="2" width="20.83203125" customWidth="1"/>
+    <col min="1" max="1" width="26.81640625" customWidth="1"/>
+    <col min="2" max="2" width="20.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -584,7 +578,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="19.25" customHeight="1">
+    <row r="2" spans="1:2" ht="19.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>17</v>
       </c>
@@ -601,454 +595,414 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J69"/>
+  <dimension ref="A1:I69"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="17.1796875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="88.6640625" customWidth="1"/>
-    <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="22.33203125" customWidth="1"/>
-    <col min="5" max="5" width="46.1640625" customWidth="1"/>
-    <col min="6" max="7" width="20" customWidth="1"/>
-    <col min="8" max="8" width="21.83203125" customWidth="1"/>
-    <col min="9" max="9" width="31.5" customWidth="1"/>
-    <col min="10" max="10" width="22.1640625" customWidth="1"/>
+    <col min="2" max="2" width="88.6328125" customWidth="1"/>
+    <col min="3" max="3" width="22.36328125" customWidth="1"/>
+    <col min="4" max="4" width="46.1796875" customWidth="1"/>
+    <col min="5" max="6" width="20" customWidth="1"/>
+    <col min="7" max="7" width="21.81640625" customWidth="1"/>
+    <col min="8" max="8" width="31.453125" customWidth="1"/>
+    <col min="9" max="9" width="22.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17.5" customHeight="1">
+    <row r="1" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>38</v>
       </c>
       <c r="B1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C1" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E1" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="G1" t="s">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="2"/>
-    </row>
-    <row r="2" spans="1:10" ht="17" customHeight="1">
+      <c r="I1" s="2"/>
+    </row>
+    <row r="2" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
       <c r="D2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="2"/>
-    </row>
-    <row r="3" spans="1:10" ht="17.5" customHeight="1">
-      <c r="F3" t="s">
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H3" t="s">
+      <c r="G3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="17" customHeight="1">
-      <c r="D4" t="s">
+    <row r="4" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
         <v>22</v>
       </c>
-      <c r="J4" s="2"/>
-    </row>
-    <row r="5" spans="1:10" ht="41" customHeight="1">
-      <c r="F5" t="s">
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" ht="41" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
         <v>2</v>
       </c>
+      <c r="G5" t="s">
+        <v>12</v>
+      </c>
       <c r="H5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="17" customHeight="1">
-      <c r="D6" t="s">
+    <row r="6" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="17" customHeight="1">
-      <c r="D7" t="s">
+    <row r="7" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="17" customHeight="1">
+    <row r="8" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B8" s="3"/>
     </row>
-    <row r="9" spans="1:10" ht="59" customHeight="1">
+    <row r="9" spans="1:9" ht="59" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" t="s">
         <v>42</v>
       </c>
-      <c r="H9" t="s">
+      <c r="G9" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="17" customHeight="1">
+    <row r="10" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
-      <c r="D10" t="s">
+      <c r="C10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="17.5" customHeight="1">
+    <row r="11" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="1:10" ht="59" customHeight="1">
+    <row r="12" spans="1:9" ht="59" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C12" t="s">
-        <v>45</v>
-      </c>
-      <c r="F12" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" t="s">
         <v>42</v>
       </c>
-      <c r="H12" t="s">
+      <c r="G12" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="17" customHeight="1">
+    <row r="13" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
-      <c r="D13" t="s">
+      <c r="C13" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="17.5" customHeight="1">
+    <row r="14" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B14" s="3"/>
     </row>
-    <row r="15" spans="1:10" ht="66" customHeight="1">
+    <row r="15" spans="1:9" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C15" t="s">
-        <v>45</v>
-      </c>
-      <c r="F15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" t="s">
         <v>42</v>
       </c>
-      <c r="H15" t="s">
+      <c r="G15" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="17" customHeight="1">
+    <row r="16" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
-      <c r="D16" t="s">
+      <c r="C16" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="17.5" customHeight="1">
+    <row r="17" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="66" customHeight="1">
+    <row r="18" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C18" t="s">
-        <v>45</v>
-      </c>
-      <c r="F18" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" t="s">
         <v>42</v>
       </c>
-      <c r="H18" t="s">
+      <c r="G18" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="17" customHeight="1">
+    <row r="19" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
-      <c r="D19" t="s">
+      <c r="C19" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="17.5" customHeight="1">
+    <row r="20" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="66" customHeight="1">
+    <row r="21" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C21" t="s">
-        <v>45</v>
-      </c>
-      <c r="F21" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" t="s">
         <v>42</v>
       </c>
-      <c r="H21" t="s">
+      <c r="G21" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="17" customHeight="1">
+    <row r="22" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
-      <c r="D22" t="s">
+      <c r="C22" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="17.5" customHeight="1">
+    <row r="23" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="66" customHeight="1">
+    <row r="24" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24" t="s">
-        <v>45</v>
-      </c>
-      <c r="F24" t="s">
+        <v>52</v>
+      </c>
+      <c r="E24" t="s">
         <v>42</v>
       </c>
-      <c r="H24" t="s">
+      <c r="G24" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="17" customHeight="1">
+    <row r="25" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
-      <c r="D25" t="s">
+      <c r="C25" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="17.5" customHeight="1">
+    <row r="26" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="66" customHeight="1">
+    <row r="27" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C27" t="s">
-        <v>45</v>
-      </c>
-      <c r="F27" t="s">
+        <v>53</v>
+      </c>
+      <c r="E27" t="s">
         <v>42</v>
       </c>
-      <c r="H27" t="s">
+      <c r="G27" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="17" customHeight="1">
+    <row r="28" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
-      <c r="D28" t="s">
+      <c r="C28" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="17.5" customHeight="1">
+    <row r="29" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="66" customHeight="1">
+    <row r="30" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C30" t="s">
-        <v>45</v>
-      </c>
-      <c r="F30" t="s">
+        <v>54</v>
+      </c>
+      <c r="E30" t="s">
         <v>42</v>
       </c>
-      <c r="H30" t="s">
+      <c r="G30" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="17" customHeight="1">
+    <row r="31" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
-      <c r="D31" t="s">
+      <c r="C31" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="17.5" customHeight="1">
+    <row r="32" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="66" customHeight="1">
+    <row r="33" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C33" t="s">
-        <v>45</v>
-      </c>
-      <c r="F33" t="s">
+        <v>55</v>
+      </c>
+      <c r="E33" t="s">
         <v>42</v>
       </c>
-      <c r="H33" t="s">
+      <c r="G33" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="17" customHeight="1">
+    <row r="34" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
-      <c r="D34" t="s">
+      <c r="C34" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="17.5" customHeight="1">
+    <row r="35" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="66" customHeight="1">
+    <row r="36" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C36" t="s">
-        <v>45</v>
-      </c>
-      <c r="F36" t="s">
+        <v>56</v>
+      </c>
+      <c r="E36" t="s">
         <v>42</v>
       </c>
-      <c r="H36" t="s">
+      <c r="G36" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="17" customHeight="1">
+    <row r="37" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
-      <c r="D37" t="s">
+      <c r="C37" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="17.5" customHeight="1">
+    <row r="38" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="66" customHeight="1">
+    <row r="39" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="B39" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C39" t="s">
-        <v>45</v>
-      </c>
-      <c r="F39" t="s">
+        <v>57</v>
+      </c>
+      <c r="E39" t="s">
         <v>42</v>
       </c>
-      <c r="H39" t="s">
+      <c r="G39" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="17" customHeight="1">
+    <row r="40" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
-      <c r="D40" t="s">
+      <c r="C40" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="17.5" customHeight="1">
+    <row r="41" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="66" customHeight="1">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C42" t="s">
-        <v>45</v>
-      </c>
-      <c r="F42" t="s">
+        <v>59</v>
+      </c>
+      <c r="E42" t="s">
         <v>42</v>
       </c>
-      <c r="H42" t="s">
+      <c r="G42" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="17" customHeight="1">
+    <row r="43" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
-      <c r="D43" t="s">
+      <c r="C43" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="17.5" customHeight="1"/>
-    <row r="45" spans="1:8" ht="17.5" customHeight="1"/>
-    <row r="46" spans="1:8" ht="17.5" customHeight="1"/>
-    <row r="47" spans="1:8" ht="17.5" customHeight="1"/>
-    <row r="48" spans="1:8" ht="17.5" customHeight="1"/>
-    <row r="49" ht="17.5" customHeight="1"/>
-    <row r="50" ht="17.5" customHeight="1"/>
-    <row r="51" ht="17.5" customHeight="1"/>
-    <row r="52" ht="17.5" customHeight="1"/>
-    <row r="53" ht="17.5" customHeight="1"/>
-    <row r="54" ht="17.5" customHeight="1"/>
-    <row r="55" ht="17.5" customHeight="1"/>
-    <row r="56" ht="17.5" customHeight="1"/>
-    <row r="57" ht="17.5" customHeight="1"/>
-    <row r="58" ht="17.5" customHeight="1"/>
-    <row r="59" ht="17.5" customHeight="1"/>
-    <row r="60" ht="17.5" customHeight="1"/>
-    <row r="61" ht="17.5" customHeight="1"/>
-    <row r="62" ht="17.5" customHeight="1"/>
-    <row r="63" ht="17.5" customHeight="1"/>
-    <row r="64" ht="17.5" customHeight="1"/>
-    <row r="65" ht="17.5" customHeight="1"/>
-    <row r="66" ht="17.5" customHeight="1"/>
-    <row r="67" ht="17.5" customHeight="1"/>
-    <row r="68" ht="17.5" customHeight="1"/>
-    <row r="69" ht="17.5" customHeight="1"/>
+    <row r="44" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1067,13 +1021,13 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="17.1796875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="24.6640625" customWidth="1"/>
-    <col min="4" max="4" width="41.33203125" customWidth="1"/>
+    <col min="3" max="3" width="24.6328125" customWidth="1"/>
+    <col min="4" max="4" width="41.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" customHeight="1">
+    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -1087,22 +1041,22 @@
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="18.75" customHeight="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="18.75" customHeight="1">
+    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1113,7 +1067,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="28" customHeight="1">
+    <row r="4" spans="1:5" ht="28" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1127,60 +1081,60 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="18.75" customHeight="1">
+    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:5" ht="18.75" customHeight="1">
+    <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:5" ht="18.75" customHeight="1"/>
-    <row r="8" spans="1:5" ht="18.75" customHeight="1"/>
-    <row r="9" spans="1:5" ht="18.75" customHeight="1">
+    <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:5" ht="18.75" customHeight="1">
+    <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:5" ht="18.75" customHeight="1">
+    <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:5" ht="18.75" customHeight="1">
+    <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
     </row>
-    <row r="15" spans="1:5" ht="12.75" customHeight="1">
+    <row r="15" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:5" ht="12.75" customHeight="1">
+    <row r="16" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:3" ht="12.75" customHeight="1">
+    <row r="17" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
     </row>
-    <row r="18" spans="1:3" ht="12.75" customHeight="1">
+    <row r="18" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
     </row>
-    <row r="21" spans="1:3" ht="12.75" customHeight="1">
+    <row r="21" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="1:3" ht="12.75" customHeight="1">
+    <row r="22" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:3" ht="12.75" customHeight="1">
+    <row r="23" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:3" ht="12.75" customHeight="1">
+    <row r="24" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
     </row>
   </sheetData>
@@ -1201,14 +1155,14 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" customWidth="1"/>
+    <col min="1" max="1" width="18.453125" customWidth="1"/>
+    <col min="2" max="2" width="22.36328125" customWidth="1"/>
     <col min="3" max="3" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -1219,7 +1173,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>27</v>
       </c>
@@ -1230,18 +1184,18 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>27</v>
       </c>
@@ -1252,7 +1206,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>27</v>
       </c>
@@ -1263,7 +1217,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>27</v>
       </c>
@@ -1274,7 +1228,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>27</v>
       </c>
@@ -1285,7 +1239,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>27</v>
       </c>
@@ -1296,7 +1250,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>27</v>
       </c>
@@ -1307,7 +1261,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>27</v>
       </c>
@@ -1318,7 +1272,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>27</v>
       </c>
@@ -1329,7 +1283,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>27</v>
       </c>
@@ -1340,15 +1294,15 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated framework to include Ethiopia Study
</commit_message>
<xml_diff>
--- a/form-files/framework/framework.xlsx
+++ b/form-files/framework/framework.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1780" yWindow="0" windowWidth="25820" windowHeight="14080" activeTab="1"/>
+    <workbookView xWindow="29220" yWindow="-27480" windowWidth="28020" windowHeight="14660" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="5" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="settings" sheetId="4" r:id="rId3"/>
     <sheet name="choices" sheetId="6" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="79">
   <si>
     <t>comments</t>
   </si>
@@ -205,13 +205,67 @@
   </si>
   <si>
     <t>showContents</t>
+  </si>
+  <si>
+    <t>Ethiopia</t>
+  </si>
+  <si>
+    <t>Ethiopia_household_data</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../tables/Ethiopia_household/forms/Ethiopia_household_data/',null)</t>
+  </si>
+  <si>
+    <t>Ethiopia_names</t>
+  </si>
+  <si>
+    <t>Ethiopia_other_info</t>
+  </si>
+  <si>
+    <t>Ethiopia_Section3</t>
+  </si>
+  <si>
+    <t>Ethiopia Section 3</t>
+  </si>
+  <si>
+    <t>Ethiopia_Section2_other_info</t>
+  </si>
+  <si>
+    <t>Ethiopia_Section2_names</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../tables/Ethiopia_members/forms/Ethiopia_Section2_names/',null)</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../tables/Ethiopia_members/forms/Ethiopia_Section2_other_info/',null)</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../tables/Ethiopia_members/forms/Ethiopia_Section3/',null)</t>
+  </si>
+  <si>
+    <t>Ethiopia_Section9_3_general</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../tables/Ethiopia_members/forms/Ethiopia_Section9_3_general/',null)</t>
+  </si>
+  <si>
+    <t>Ethiopia_Section9_3_injuries</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../tables/Ethiopia_members/forms/Ethiopia_Section9_3_injuries/',null)</t>
+  </si>
+  <si>
+    <t>Ethiopia Section 9.3 general</t>
+  </si>
+  <si>
+    <t>Ethiopia Section 9.3 Injuries</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -220,6 +274,18 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -240,8 +306,38 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -258,7 +354,37 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="31">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -564,13 +690,13 @@
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="26.81640625" customWidth="1"/>
-    <col min="2" max="2" width="20.81640625" customWidth="1"/>
+    <col min="1" max="1" width="26.83203125" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -578,7 +704,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="19.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="19.25" customHeight="1">
       <c r="B2" t="s">
         <v>17</v>
       </c>
@@ -595,24 +721,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I69"/>
+  <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44:XFD61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.1796875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="88.6328125" customWidth="1"/>
-    <col min="3" max="3" width="22.36328125" customWidth="1"/>
-    <col min="4" max="4" width="46.1796875" customWidth="1"/>
+    <col min="2" max="2" width="101.1640625" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="4" max="4" width="46.1640625" customWidth="1"/>
     <col min="5" max="6" width="20" customWidth="1"/>
-    <col min="7" max="7" width="21.81640625" customWidth="1"/>
-    <col min="8" max="8" width="31.453125" customWidth="1"/>
-    <col min="9" max="9" width="22.1796875" customWidth="1"/>
+    <col min="7" max="7" width="21.83203125" customWidth="1"/>
+    <col min="8" max="8" width="31.5" customWidth="1"/>
+    <col min="9" max="9" width="22.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="17.5" customHeight="1">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -639,7 +765,7 @@
       </c>
       <c r="I1" s="2"/>
     </row>
-    <row r="2" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="17" customHeight="1">
       <c r="C2" t="s">
         <v>20</v>
       </c>
@@ -648,7 +774,7 @@
       </c>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="17.5" customHeight="1">
       <c r="E3" t="s">
         <v>24</v>
       </c>
@@ -659,13 +785,13 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="17" customHeight="1">
       <c r="C4" t="s">
         <v>22</v>
       </c>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:9" ht="41" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="41" customHeight="1">
       <c r="E5" t="s">
         <v>2</v>
       </c>
@@ -676,23 +802,23 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="17" customHeight="1">
       <c r="C6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="17" customHeight="1">
       <c r="C7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="17" customHeight="1">
       <c r="A8" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B8" s="3"/>
     </row>
-    <row r="9" spans="1:9" ht="59" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="59" customHeight="1">
       <c r="A9" s="3"/>
       <c r="B9" s="4" t="s">
         <v>47</v>
@@ -704,20 +830,20 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="17" customHeight="1">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="17.5" customHeight="1">
       <c r="A11" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="1:9" ht="59" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="59" customHeight="1">
       <c r="A12" s="3"/>
       <c r="B12" s="4" t="s">
         <v>48</v>
@@ -729,20 +855,20 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="17" customHeight="1">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="17.5" customHeight="1">
       <c r="A14" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B14" s="3"/>
     </row>
-    <row r="15" spans="1:9" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="66" customHeight="1">
       <c r="A15" s="3"/>
       <c r="B15" s="4" t="s">
         <v>49</v>
@@ -754,19 +880,19 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="17" customHeight="1">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="17.5" customHeight="1">
       <c r="A17" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="66" customHeight="1">
       <c r="A18" s="3"/>
       <c r="B18" s="4" t="s">
         <v>50</v>
@@ -778,19 +904,19 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="17" customHeight="1">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="17.5" customHeight="1">
       <c r="A20" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="66" customHeight="1">
       <c r="A21" s="3"/>
       <c r="B21" s="4" t="s">
         <v>51</v>
@@ -802,19 +928,19 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="17" customHeight="1">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="17.5" customHeight="1">
       <c r="A23" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="66" customHeight="1">
       <c r="A24" s="3"/>
       <c r="B24" s="4" t="s">
         <v>52</v>
@@ -826,19 +952,19 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="17" customHeight="1">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="17.5" customHeight="1">
       <c r="A26" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="66" customHeight="1">
       <c r="A27" s="3"/>
       <c r="B27" s="4" t="s">
         <v>53</v>
@@ -850,19 +976,19 @@
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="17" customHeight="1">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="17.5" customHeight="1">
       <c r="A29" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="66" customHeight="1">
       <c r="A30" s="3"/>
       <c r="B30" s="4" t="s">
         <v>54</v>
@@ -874,19 +1000,19 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="17" customHeight="1">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="17.5" customHeight="1">
       <c r="A32" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="66" customHeight="1">
       <c r="A33" s="3"/>
       <c r="B33" s="4" t="s">
         <v>55</v>
@@ -898,19 +1024,19 @@
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="17" customHeight="1">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="17.5" customHeight="1">
       <c r="A35" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="66" customHeight="1">
       <c r="A36" s="3"/>
       <c r="B36" s="4" t="s">
         <v>56</v>
@@ -922,19 +1048,19 @@
         <v>43</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="17" customHeight="1">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="17.5" customHeight="1">
       <c r="A38" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="66" customHeight="1">
       <c r="A39" s="3"/>
       <c r="B39" s="4" t="s">
         <v>57</v>
@@ -946,19 +1072,19 @@
         <v>43</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="17" customHeight="1">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="17.5" customHeight="1">
       <c r="A41" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="66" customHeight="1">
       <c r="A42" s="3"/>
       <c r="B42" s="4" t="s">
         <v>59</v>
@@ -970,41 +1096,145 @@
         <v>43</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="17" customHeight="1">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="65" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="66" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="67" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="68" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="69" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:7" ht="31" customHeight="1">
+      <c r="A44" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="66" customHeight="1">
+      <c r="A45" s="3"/>
+      <c r="B45" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E45" t="s">
+        <v>42</v>
+      </c>
+      <c r="G45" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="17" customHeight="1">
+      <c r="A46" s="3"/>
+      <c r="B46" s="3"/>
+      <c r="C46" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="31" customHeight="1">
+      <c r="A47" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="17.5" customHeight="1">
+      <c r="B48" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E48" t="s">
+        <v>42</v>
+      </c>
+      <c r="G48" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="17.5" customHeight="1">
+      <c r="C49" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="33" customHeight="1">
+      <c r="A50" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="17.5" customHeight="1">
+      <c r="B51" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E51" t="s">
+        <v>42</v>
+      </c>
+      <c r="G51" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="17.5" customHeight="1">
+      <c r="C52" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="26" customHeight="1">
+      <c r="A53" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="12.75" customHeight="1">
+      <c r="B54" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E54" t="s">
+        <v>42</v>
+      </c>
+      <c r="G54" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="16" customHeight="1">
+      <c r="C55" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A56" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="12.75" customHeight="1">
+      <c r="B57" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E57" t="s">
+        <v>42</v>
+      </c>
+      <c r="G57" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="12.75" customHeight="1">
+      <c r="C58" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A59" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="12.75" customHeight="1">
+      <c r="B60" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E60" t="s">
+        <v>42</v>
+      </c>
+      <c r="G60" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="12.75" customHeight="1">
+      <c r="C61" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1018,16 +1248,16 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.1796875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="3" width="24.6328125" customWidth="1"/>
-    <col min="4" max="4" width="41.36328125" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" customWidth="1"/>
+    <col min="4" max="4" width="41.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="18.75" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -1044,7 +1274,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="18.75" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1056,7 +1286,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="18.75" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1067,7 +1297,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="28" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="28" customHeight="1">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1081,60 +1311,60 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="18.75" customHeight="1">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="18.75" customHeight="1">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="18.75" customHeight="1"/>
+    <row r="8" spans="1:5" ht="18.75" customHeight="1"/>
+    <row r="9" spans="1:5" ht="18.75" customHeight="1">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="18.75" customHeight="1">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="18.75" customHeight="1">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="18.75" customHeight="1">
       <c r="A12" s="1"/>
     </row>
-    <row r="15" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="12.75" customHeight="1">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="12.75" customHeight="1">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="12.75" customHeight="1">
       <c r="A17" s="1"/>
     </row>
-    <row r="18" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="12.75" customHeight="1">
       <c r="A18" s="1"/>
     </row>
-    <row r="21" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="12.75" customHeight="1">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="12.75" customHeight="1">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="12.75" customHeight="1">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="12.75" customHeight="1">
       <c r="A24" s="1"/>
     </row>
   </sheetData>
@@ -1149,20 +1379,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.453125" customWidth="1"/>
-    <col min="2" max="2" width="22.36328125" customWidth="1"/>
+    <col min="1" max="1" width="18.5" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" customWidth="1"/>
     <col min="3" max="3" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -1173,7 +1403,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
         <v>27</v>
       </c>
@@ -1184,7 +1414,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="3" t="s">
         <v>27</v>
       </c>
@@ -1195,7 +1425,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="3" t="s">
         <v>27</v>
       </c>
@@ -1206,7 +1436,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
         <v>27</v>
       </c>
@@ -1217,7 +1447,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" s="3" t="s">
         <v>27</v>
       </c>
@@ -1228,7 +1458,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" s="3" t="s">
         <v>27</v>
       </c>
@@ -1239,7 +1469,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" s="3" t="s">
         <v>27</v>
       </c>
@@ -1250,7 +1480,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" s="3" t="s">
         <v>27</v>
       </c>
@@ -1261,7 +1491,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" s="3" t="s">
         <v>27</v>
       </c>
@@ -1272,7 +1502,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" s="3" t="s">
         <v>27</v>
       </c>
@@ -1283,7 +1513,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" s="3" t="s">
         <v>27</v>
       </c>
@@ -1294,7 +1524,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="A13" s="3" t="s">
         <v>27</v>
       </c>
@@ -1304,6 +1534,75 @@
       <c r="C13" t="s">
         <v>58</v>
       </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="24">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="24">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="24">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Removed old Ethiopia forms and added new Demo ones to showcase subforms and linked table selects.
</commit_message>
<xml_diff>
--- a/form-files/framework/framework.xlsx
+++ b/form-files/framework/framework.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="29220" yWindow="-27480" windowWidth="28020" windowHeight="14660" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="5" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="73">
   <si>
     <t>comments</t>
   </si>
@@ -213,52 +213,34 @@
     <t>Ethiopia_household_data</t>
   </si>
   <si>
-    <t>'?' + opendatakit.getHashString('../tables/Ethiopia_household/forms/Ethiopia_household_data/',null)</t>
-  </si>
-  <si>
     <t>Ethiopia_names</t>
   </si>
   <si>
     <t>Ethiopia_other_info</t>
   </si>
   <si>
-    <t>Ethiopia_Section3</t>
-  </si>
-  <si>
-    <t>Ethiopia Section 3</t>
-  </si>
-  <si>
     <t>Ethiopia_Section2_other_info</t>
   </si>
   <si>
     <t>Ethiopia_Section2_names</t>
   </si>
   <si>
-    <t>'?' + opendatakit.getHashString('../tables/Ethiopia_members/forms/Ethiopia_Section2_names/',null)</t>
-  </si>
-  <si>
-    <t>'?' + opendatakit.getHashString('../tables/Ethiopia_members/forms/Ethiopia_Section2_other_info/',null)</t>
-  </si>
-  <si>
-    <t>'?' + opendatakit.getHashString('../tables/Ethiopia_members/forms/Ethiopia_Section3/',null)</t>
-  </si>
-  <si>
-    <t>Ethiopia_Section9_3_general</t>
-  </si>
-  <si>
-    <t>'?' + opendatakit.getHashString('../tables/Ethiopia_members/forms/Ethiopia_Section9_3_general/',null)</t>
-  </si>
-  <si>
-    <t>Ethiopia_Section9_3_injuries</t>
-  </si>
-  <si>
-    <t>'?' + opendatakit.getHashString('../tables/Ethiopia_members/forms/Ethiopia_Section9_3_injuries/',null)</t>
-  </si>
-  <si>
-    <t>Ethiopia Section 9.3 general</t>
-  </si>
-  <si>
-    <t>Ethiopia Section 9.3 Injuries</t>
+    <t>Ethiopia_Section4</t>
+  </si>
+  <si>
+    <t>Ethiopia Section 4</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../tables/Ethiopia_Demo_Household/forms/Ethiopia_household_data/',null)</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../tables/Ethiopia_Demo_Members/forms/Ethiopia_Section2_names/',null)</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../tables/Ethiopia_Demo_Members/forms/Ethiopia_Section2_other_info/',null)</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../tables/Ethiopia_Demo_Members/forms/Ethiopia_Section4/',null)</t>
   </si>
 </sst>
 </file>
@@ -306,8 +288,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -354,7 +348,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="31">
+  <cellStyles count="43">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -370,6 +364,12 @@
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -385,6 +385,12 @@
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -721,10 +727,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I61"/>
+  <dimension ref="A1:I55"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44:XFD61"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1111,7 +1117,7 @@
     <row r="45" spans="1:7" ht="66" customHeight="1">
       <c r="A45" s="3"/>
       <c r="B45" s="4" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="E45" t="s">
         <v>42</v>
@@ -1129,7 +1135,7 @@
     </row>
     <row r="47" spans="1:7" ht="31" customHeight="1">
       <c r="A47" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="17.5" customHeight="1">
@@ -1150,7 +1156,7 @@
     </row>
     <row r="50" spans="1:7" ht="33" customHeight="1">
       <c r="A50" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="17.5" customHeight="1">
@@ -1169,12 +1175,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="26" customHeight="1">
+    <row r="53" spans="1:7" ht="16" customHeight="1">
       <c r="A53" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="12.75" customHeight="1">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="16" customHeight="1">
       <c r="B54" s="4" t="s">
         <v>72</v>
       </c>
@@ -1187,48 +1193,6 @@
     </row>
     <row r="55" spans="1:7" ht="16" customHeight="1">
       <c r="C55" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A56" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" ht="12.75" customHeight="1">
-      <c r="B57" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E57" t="s">
-        <v>42</v>
-      </c>
-      <c r="G57" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" ht="12.75" customHeight="1">
-      <c r="C58" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" ht="12.75" customHeight="1">
-      <c r="A59" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" ht="12.75" customHeight="1">
-      <c r="B60" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E60" t="s">
-        <v>42</v>
-      </c>
-      <c r="G60" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" ht="12.75" customHeight="1">
-      <c r="C61" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1379,9 +1343,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -1551,10 +1515,10 @@
         <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="24">
@@ -1562,10 +1526,10 @@
         <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1573,36 +1537,11 @@
         <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C17" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="24">
-      <c r="A18" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" t="s">
-        <v>73</v>
-      </c>
-      <c r="C18" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="24">
-      <c r="A19" t="s">
-        <v>27</v>
-      </c>
-      <c r="B19" t="s">
-        <v>75</v>
-      </c>
-      <c r="C19" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="3"/>
+        <v>68</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
removed ethiopia demo forms
</commit_message>
<xml_diff>
--- a/form-files/framework/framework.xlsx
+++ b/form-files/framework/framework.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="5" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="61">
   <si>
     <t>comments</t>
   </si>
@@ -205,42 +205,6 @@
   </si>
   <si>
     <t>showContents</t>
-  </si>
-  <si>
-    <t>Ethiopia</t>
-  </si>
-  <si>
-    <t>Ethiopia_household_data</t>
-  </si>
-  <si>
-    <t>Ethiopia_names</t>
-  </si>
-  <si>
-    <t>Ethiopia_other_info</t>
-  </si>
-  <si>
-    <t>Ethiopia_Section2_other_info</t>
-  </si>
-  <si>
-    <t>Ethiopia_Section2_names</t>
-  </si>
-  <si>
-    <t>Ethiopia_Section4</t>
-  </si>
-  <si>
-    <t>Ethiopia Section 4</t>
-  </si>
-  <si>
-    <t>'?' + opendatakit.getHashString('../tables/Ethiopia_Demo_Household/forms/Ethiopia_household_data/',null)</t>
-  </si>
-  <si>
-    <t>'?' + opendatakit.getHashString('../tables/Ethiopia_Demo_Members/forms/Ethiopia_Section2_names/',null)</t>
-  </si>
-  <si>
-    <t>'?' + opendatakit.getHashString('../tables/Ethiopia_Demo_Members/forms/Ethiopia_Section2_other_info/',null)</t>
-  </si>
-  <si>
-    <t>'?' + opendatakit.getHashString('../tables/Ethiopia_Demo_Members/forms/Ethiopia_Section4/',null)</t>
   </si>
 </sst>
 </file>
@@ -727,10 +691,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I55"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1106,93 +1070,6 @@
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="31" customHeight="1">
-      <c r="A44" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="66" customHeight="1">
-      <c r="A45" s="3"/>
-      <c r="B45" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E45" t="s">
-        <v>42</v>
-      </c>
-      <c r="G45" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="17" customHeight="1">
-      <c r="A46" s="3"/>
-      <c r="B46" s="3"/>
-      <c r="C46" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="31" customHeight="1">
-      <c r="A47" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="17.5" customHeight="1">
-      <c r="B48" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E48" t="s">
-        <v>42</v>
-      </c>
-      <c r="G48" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="17.5" customHeight="1">
-      <c r="C49" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="33" customHeight="1">
-      <c r="A50" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="17.5" customHeight="1">
-      <c r="B51" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="E51" t="s">
-        <v>42</v>
-      </c>
-      <c r="G51" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="17.5" customHeight="1">
-      <c r="C52" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="16" customHeight="1">
-      <c r="A53" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="16" customHeight="1">
-      <c r="B54" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="E54" t="s">
-        <v>42</v>
-      </c>
-      <c r="G54" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" ht="16" customHeight="1">
-      <c r="C55" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1343,10 +1220,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1499,50 +1376,6 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" t="s">
-        <v>62</v>
-      </c>
-      <c r="C14" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" t="s">
-        <v>66</v>
-      </c>
-      <c r="C15" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="24">
-      <c r="A16" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" t="s">
-        <v>65</v>
-      </c>
-      <c r="C16" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" t="s">
-        <v>67</v>
-      </c>
-      <c r="C17" t="s">
-        <v>68</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
added the rest of the forms
</commit_message>
<xml_diff>
--- a/form-files/framework/framework.xlsx
+++ b/form-files/framework/framework.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="29220" yWindow="-27480" windowWidth="28020" windowHeight="14660" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="5" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="109">
   <si>
     <t>comments</t>
   </si>
@@ -213,52 +213,142 @@
     <t>Ethiopia_household_data</t>
   </si>
   <si>
+    <t>Ethiopia_names</t>
+  </si>
+  <si>
+    <t>Ethiopia_other_info</t>
+  </si>
+  <si>
+    <t>Ethiopia_Section2_other_info</t>
+  </si>
+  <si>
+    <t>Ethiopia_Section2_names</t>
+  </si>
+  <si>
+    <t>Ethiopia_Section4</t>
+  </si>
+  <si>
+    <t>Ethiopia Section 4</t>
+  </si>
+  <si>
     <t>'?' + opendatakit.getHashString('../tables/Ethiopia_household/forms/Ethiopia_household_data/',null)</t>
   </si>
   <si>
-    <t>Ethiopia_names</t>
-  </si>
-  <si>
-    <t>Ethiopia_other_info</t>
+    <t>'?' + opendatakit.getHashString('../tables/Ethiopia_members/forms/Ethiopia_Section2_names/',null)</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../tables/Ethiopia_members/forms/Ethiopia_Section2_other_info/',null)</t>
   </si>
   <si>
     <t>Ethiopia_Section3</t>
   </si>
   <si>
-    <t>Ethiopia Section 3</t>
-  </si>
-  <si>
-    <t>Ethiopia_Section2_other_info</t>
-  </si>
-  <si>
-    <t>Ethiopia_Section2_names</t>
-  </si>
-  <si>
-    <t>'?' + opendatakit.getHashString('../tables/Ethiopia_members/forms/Ethiopia_Section2_names/',null)</t>
-  </si>
-  <si>
-    <t>'?' + opendatakit.getHashString('../tables/Ethiopia_members/forms/Ethiopia_Section2_other_info/',null)</t>
-  </si>
-  <si>
     <t>'?' + opendatakit.getHashString('../tables/Ethiopia_members/forms/Ethiopia_Section3/',null)</t>
   </si>
   <si>
-    <t>Ethiopia_Section9_3_general</t>
-  </si>
-  <si>
-    <t>'?' + opendatakit.getHashString('../tables/Ethiopia_members/forms/Ethiopia_Section9_3_general/',null)</t>
-  </si>
-  <si>
-    <t>Ethiopia_Section9_3_injuries</t>
-  </si>
-  <si>
-    <t>'?' + opendatakit.getHashString('../tables/Ethiopia_members/forms/Ethiopia_Section9_3_injuries/',null)</t>
-  </si>
-  <si>
-    <t>Ethiopia Section 9.3 general</t>
-  </si>
-  <si>
-    <t>Ethiopia Section 9.3 Injuries</t>
+    <t>'?' + opendatakit.getHashString('../tables/Ethiopia_members/forms/Ethiopia_Section4/',null)</t>
+  </si>
+  <si>
+    <t>Ethiopia_Section5</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../tables/Ethiopia_members/forms/Ethiopia_Section5/',null)</t>
+  </si>
+  <si>
+    <t>Ethiopia_Section82</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../tables/Ethiopia_members/forms/Ethiopia_Section82/',null)</t>
+  </si>
+  <si>
+    <t>Ethiopia_Section82_p2</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../tables/Ethiopia_members/forms/Ethiopia_Section82_p2/',null)</t>
+  </si>
+  <si>
+    <t>Ethiopia_Section82_p3</t>
+  </si>
+  <si>
+    <t>Ethiopia_Section82_p4</t>
+  </si>
+  <si>
+    <t>Ethiopia_Section82_p5</t>
+  </si>
+  <si>
+    <t>Ethiopia Section 5</t>
+  </si>
+  <si>
+    <t>Ethiopia Section 8.2</t>
+  </si>
+  <si>
+    <t>Ethiopia Section 8.2 p2</t>
+  </si>
+  <si>
+    <t>Ethiopia_Section91</t>
+  </si>
+  <si>
+    <t>Ethiopia_Section91_p2</t>
+  </si>
+  <si>
+    <t>Ethiopia Section 8.2 p3</t>
+  </si>
+  <si>
+    <t>Ethiopia Section 8.2 p4</t>
+  </si>
+  <si>
+    <t>Ethiopia Section 8.2 p5</t>
+  </si>
+  <si>
+    <t>Ethiopia Section 9.1</t>
+  </si>
+  <si>
+    <t>Ethiopia Section 9.1 p2</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../tables/Ethiopia_members/forms/Ethiopia_Section82_p3/',null)</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../tables/Ethiopia_members/forms/Ethiopia_Section82_p4/',null)</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../tables/Ethiopia_members/forms/Ethiopia_Section82_p5/',null)</t>
+  </si>
+  <si>
+    <t>Ethiopia_Section93</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../tables/Ethiopia_members/forms/Ethiopia_Section93/',null)</t>
+  </si>
+  <si>
+    <t>Ethiopia_Section93_p2</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../tables/Ethiopia_members/forms/Ethiopia_Section93_p2/',null)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ethiopia Section 9.3 </t>
+  </si>
+  <si>
+    <t>Ethiopia Section 9.3 p2</t>
+  </si>
+  <si>
+    <t>Ethiopia_Section94</t>
+  </si>
+  <si>
+    <t>Ethiopia Section 9.4</t>
+  </si>
+  <si>
+    <t>Ethiopia_Section95</t>
+  </si>
+  <si>
+    <t>Ethiopia Section 9.5</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../tables/Ethiopia_members/forms/Ethiopia_Section94/',null)</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../tables/Ethiopia_members/forms/Ethiopia_Section95/',null)</t>
   </si>
 </sst>
 </file>
@@ -306,8 +396,38 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -354,7 +474,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="31">
+  <cellStyles count="61">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -370,6 +490,21 @@
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -385,6 +520,21 @@
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -721,10 +871,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I61"/>
+  <dimension ref="A1:I88"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44:XFD61"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="B88" sqref="B88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1111,7 +1261,7 @@
     <row r="45" spans="1:7" ht="66" customHeight="1">
       <c r="A45" s="3"/>
       <c r="B45" s="4" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="E45" t="s">
         <v>42</v>
@@ -1129,7 +1279,7 @@
     </row>
     <row r="47" spans="1:7" ht="31" customHeight="1">
       <c r="A47" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="17.5" customHeight="1">
@@ -1150,7 +1300,7 @@
     </row>
     <row r="50" spans="1:7" ht="33" customHeight="1">
       <c r="A50" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="17.5" customHeight="1">
@@ -1169,14 +1319,14 @@
         <v>41</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="26" customHeight="1">
+    <row r="53" spans="1:7" ht="16" customHeight="1">
       <c r="A53" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="12.75" customHeight="1">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="16" customHeight="1">
       <c r="B54" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E54" t="s">
         <v>42</v>
@@ -1190,12 +1340,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="12.75" customHeight="1">
+    <row r="56" spans="1:7" ht="16" customHeight="1">
       <c r="A56" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" ht="12.75" customHeight="1">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="16" customHeight="1">
       <c r="B57" s="4" t="s">
         <v>74</v>
       </c>
@@ -1206,17 +1356,17 @@
         <v>43</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="12.75" customHeight="1">
+    <row r="58" spans="1:7" ht="16" customHeight="1">
       <c r="C58" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="12.75" customHeight="1">
+    <row r="59" spans="1:7" ht="16" customHeight="1">
       <c r="A59" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="12.75" customHeight="1">
+    <row r="60" spans="1:7" ht="16" customHeight="1">
       <c r="B60" s="4" t="s">
         <v>76</v>
       </c>
@@ -1227,8 +1377,197 @@
         <v>43</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="12.75" customHeight="1">
+    <row r="61" spans="1:7" ht="16" customHeight="1">
       <c r="C61" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="16" customHeight="1">
+      <c r="A62" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="16" customHeight="1">
+      <c r="B63" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E63" t="s">
+        <v>42</v>
+      </c>
+      <c r="G63" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="16" customHeight="1">
+      <c r="C64" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="16" customHeight="1">
+      <c r="A65" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="16" customHeight="1">
+      <c r="B66" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E66" t="s">
+        <v>42</v>
+      </c>
+      <c r="G66" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="16" customHeight="1">
+      <c r="C67" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A68" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="12.75" customHeight="1">
+      <c r="B69" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E69" t="s">
+        <v>42</v>
+      </c>
+      <c r="G69" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="12.75" customHeight="1">
+      <c r="C70" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A71" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="12.75" customHeight="1">
+      <c r="B72" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E72" t="s">
+        <v>42</v>
+      </c>
+      <c r="G72" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="13" customHeight="1">
+      <c r="C73" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A74" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="12.75" customHeight="1">
+      <c r="B75" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E75" t="s">
+        <v>42</v>
+      </c>
+      <c r="G75" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="12.75" customHeight="1">
+      <c r="C76" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A77" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="12.75" customHeight="1">
+      <c r="B78" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E78" t="s">
+        <v>42</v>
+      </c>
+      <c r="G78" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="12.75" customHeight="1">
+      <c r="C79" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A80" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="12.75" customHeight="1">
+      <c r="B81" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E81" t="s">
+        <v>42</v>
+      </c>
+      <c r="G81" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="12.75" customHeight="1">
+      <c r="C82" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A83" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="12.75" customHeight="1">
+      <c r="B84" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E84" t="s">
+        <v>42</v>
+      </c>
+      <c r="G84" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="12.75" customHeight="1">
+      <c r="C85" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A86" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="12.75" customHeight="1">
+      <c r="B87" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="E87" t="s">
+        <v>42</v>
+      </c>
+      <c r="G87" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="12.75" customHeight="1">
+      <c r="C88" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1379,10 +1718,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1551,10 +1890,10 @@
         <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="24">
@@ -1562,10 +1901,10 @@
         <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1573,36 +1912,143 @@
         <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C17" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="24">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>27</v>
       </c>
       <c r="B18" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="24">
-      <c r="A19" t="s">
-        <v>27</v>
-      </c>
-      <c r="B19" t="s">
-        <v>75</v>
-      </c>
       <c r="C19" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="3"/>
+      <c r="A20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" t="s">
+        <v>82</v>
+      </c>
+      <c r="C22" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" t="s">
+        <v>83</v>
+      </c>
+      <c r="C23" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" t="s">
+        <v>87</v>
+      </c>
+      <c r="C24" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" t="s">
+        <v>88</v>
+      </c>
+      <c r="C25" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" t="s">
+        <v>97</v>
+      </c>
+      <c r="C26" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" t="s">
+        <v>99</v>
+      </c>
+      <c r="C27" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>103</v>
+      </c>
+      <c r="C28" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>105</v>
+      </c>
+      <c r="C29" t="s">
+        <v>106</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>